<commit_message>
scrape url each activities.r1
</commit_message>
<xml_diff>
--- a/results/result.xlsx
+++ b/results/result.xlsx
@@ -443,140 +443,140 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>https://www.airbnb.com/experiences/132375?currentTab=experience_tab&amp;federatedSearchId=526f5db2-2cae-4623-ac66-a5a254ae550c&amp;searchId=10e5ef69-49a1-4355-8dd6-d4fbd63addef&amp;sectionId=8d95b00f-bf58-4e5e-bb2a-cd27e7f450cc</t>
+          <t>https://www.airbnb.com/experiences/132375?currentTab=experience_tab&amp;federatedSearchId=e74343bc-d4f2-44b5-bcbb-261b1bd0e7d3&amp;searchId=b06b2908-16d1-40ae-a1bb-0864f164d27b&amp;sectionId=7f116f53-1a8d-42d9-a67a-0055d302498a</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>https://www.airbnb.com/experiences/280110?currentTab=experience_tab&amp;federatedSearchId=526f5db2-2cae-4623-ac66-a5a254ae550c&amp;searchId=10e5ef69-49a1-4355-8dd6-d4fbd63addef&amp;sectionId=8d95b00f-bf58-4e5e-bb2a-cd27e7f450cc</t>
+          <t>https://www.airbnb.com/experiences/280110?currentTab=experience_tab&amp;federatedSearchId=e74343bc-d4f2-44b5-bcbb-261b1bd0e7d3&amp;searchId=b06b2908-16d1-40ae-a1bb-0864f164d27b&amp;sectionId=7f116f53-1a8d-42d9-a67a-0055d302498a</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>https://www.airbnb.com/experiences/3403346?currentTab=experience_tab&amp;federatedSearchId=526f5db2-2cae-4623-ac66-a5a254ae550c&amp;searchId=10e5ef69-49a1-4355-8dd6-d4fbd63addef&amp;sectionId=8d95b00f-bf58-4e5e-bb2a-cd27e7f450cc</t>
+          <t>https://www.airbnb.com/experiences/3403346?currentTab=experience_tab&amp;federatedSearchId=e74343bc-d4f2-44b5-bcbb-261b1bd0e7d3&amp;searchId=b06b2908-16d1-40ae-a1bb-0864f164d27b&amp;sectionId=7f116f53-1a8d-42d9-a67a-0055d302498a</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>https://www.airbnb.com/experiences/2189069?currentTab=experience_tab&amp;federatedSearchId=526f5db2-2cae-4623-ac66-a5a254ae550c&amp;searchId=10e5ef69-49a1-4355-8dd6-d4fbd63addef&amp;sectionId=8d95b00f-bf58-4e5e-bb2a-cd27e7f450cc</t>
+          <t>https://www.airbnb.com/experiences/2189069?currentTab=experience_tab&amp;federatedSearchId=e74343bc-d4f2-44b5-bcbb-261b1bd0e7d3&amp;searchId=b06b2908-16d1-40ae-a1bb-0864f164d27b&amp;sectionId=7f116f53-1a8d-42d9-a67a-0055d302498a</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>https://www.airbnb.com/experiences/236040?currentTab=experience_tab&amp;federatedSearchId=526f5db2-2cae-4623-ac66-a5a254ae550c&amp;searchId=10e5ef69-49a1-4355-8dd6-d4fbd63addef&amp;sectionId=8d95b00f-bf58-4e5e-bb2a-cd27e7f450cc</t>
+          <t>https://www.airbnb.com/experiences/236040?currentTab=experience_tab&amp;federatedSearchId=e74343bc-d4f2-44b5-bcbb-261b1bd0e7d3&amp;searchId=b06b2908-16d1-40ae-a1bb-0864f164d27b&amp;sectionId=7f116f53-1a8d-42d9-a67a-0055d302498a</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>https://www.airbnb.com/experiences/175656?currentTab=experience_tab&amp;federatedSearchId=526f5db2-2cae-4623-ac66-a5a254ae550c&amp;searchId=10e5ef69-49a1-4355-8dd6-d4fbd63addef&amp;sectionId=8d95b00f-bf58-4e5e-bb2a-cd27e7f450cc</t>
+          <t>https://www.airbnb.com/experiences/175656?currentTab=experience_tab&amp;federatedSearchId=e74343bc-d4f2-44b5-bcbb-261b1bd0e7d3&amp;searchId=b06b2908-16d1-40ae-a1bb-0864f164d27b&amp;sectionId=7f116f53-1a8d-42d9-a67a-0055d302498a</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>https://www.airbnb.com/experiences/2953268?currentTab=experience_tab&amp;federatedSearchId=526f5db2-2cae-4623-ac66-a5a254ae550c&amp;searchId=10e5ef69-49a1-4355-8dd6-d4fbd63addef&amp;sectionId=8d95b00f-bf58-4e5e-bb2a-cd27e7f450cc</t>
+          <t>https://www.airbnb.com/experiences/2953268?currentTab=experience_tab&amp;federatedSearchId=e74343bc-d4f2-44b5-bcbb-261b1bd0e7d3&amp;searchId=b06b2908-16d1-40ae-a1bb-0864f164d27b&amp;sectionId=7f116f53-1a8d-42d9-a67a-0055d302498a</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>https://www.airbnb.com/experiences/225309?currentTab=experience_tab&amp;federatedSearchId=526f5db2-2cae-4623-ac66-a5a254ae550c&amp;searchId=10e5ef69-49a1-4355-8dd6-d4fbd63addef&amp;sectionId=8d95b00f-bf58-4e5e-bb2a-cd27e7f450cc</t>
+          <t>https://www.airbnb.com/experiences/225309?currentTab=experience_tab&amp;federatedSearchId=e74343bc-d4f2-44b5-bcbb-261b1bd0e7d3&amp;searchId=b06b2908-16d1-40ae-a1bb-0864f164d27b&amp;sectionId=7f116f53-1a8d-42d9-a67a-0055d302498a</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>https://www.airbnb.com/experiences/4262536?currentTab=experience_tab&amp;federatedSearchId=526f5db2-2cae-4623-ac66-a5a254ae550c&amp;searchId=10e5ef69-49a1-4355-8dd6-d4fbd63addef&amp;sectionId=8d95b00f-bf58-4e5e-bb2a-cd27e7f450cc</t>
+          <t>https://www.airbnb.com/experiences/4262536?currentTab=experience_tab&amp;federatedSearchId=e74343bc-d4f2-44b5-bcbb-261b1bd0e7d3&amp;searchId=b06b2908-16d1-40ae-a1bb-0864f164d27b&amp;sectionId=7f116f53-1a8d-42d9-a67a-0055d302498a</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>https://www.airbnb.com/experiences/513872?currentTab=experience_tab&amp;federatedSearchId=526f5db2-2cae-4623-ac66-a5a254ae550c&amp;searchId=10e5ef69-49a1-4355-8dd6-d4fbd63addef&amp;sectionId=8d95b00f-bf58-4e5e-bb2a-cd27e7f450cc</t>
+          <t>https://www.airbnb.com/experiences/513872?currentTab=experience_tab&amp;federatedSearchId=e74343bc-d4f2-44b5-bcbb-261b1bd0e7d3&amp;searchId=b06b2908-16d1-40ae-a1bb-0864f164d27b&amp;sectionId=7f116f53-1a8d-42d9-a67a-0055d302498a</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>https://www.airbnb.com/experiences/3584422?currentTab=experience_tab&amp;federatedSearchId=526f5db2-2cae-4623-ac66-a5a254ae550c&amp;searchId=10e5ef69-49a1-4355-8dd6-d4fbd63addef&amp;sectionId=8d95b00f-bf58-4e5e-bb2a-cd27e7f450cc</t>
+          <t>https://www.airbnb.com/experiences/3584422?currentTab=experience_tab&amp;federatedSearchId=e74343bc-d4f2-44b5-bcbb-261b1bd0e7d3&amp;searchId=b06b2908-16d1-40ae-a1bb-0864f164d27b&amp;sectionId=7f116f53-1a8d-42d9-a67a-0055d302498a</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>https://www.airbnb.com/experiences/427945?currentTab=experience_tab&amp;federatedSearchId=526f5db2-2cae-4623-ac66-a5a254ae550c&amp;searchId=10e5ef69-49a1-4355-8dd6-d4fbd63addef&amp;sectionId=8d95b00f-bf58-4e5e-bb2a-cd27e7f450cc</t>
+          <t>https://www.airbnb.com/experiences/427945?currentTab=experience_tab&amp;federatedSearchId=e74343bc-d4f2-44b5-bcbb-261b1bd0e7d3&amp;searchId=b06b2908-16d1-40ae-a1bb-0864f164d27b&amp;sectionId=7f116f53-1a8d-42d9-a67a-0055d302498a</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>https://www.airbnb.com/experiences/2046187?currentTab=experience_tab&amp;federatedSearchId=526f5db2-2cae-4623-ac66-a5a254ae550c&amp;searchId=10e5ef69-49a1-4355-8dd6-d4fbd63addef&amp;sectionId=8d95b00f-bf58-4e5e-bb2a-cd27e7f450cc</t>
+          <t>https://www.airbnb.com/experiences/2046187?currentTab=experience_tab&amp;federatedSearchId=e74343bc-d4f2-44b5-bcbb-261b1bd0e7d3&amp;searchId=b06b2908-16d1-40ae-a1bb-0864f164d27b&amp;sectionId=7f116f53-1a8d-42d9-a67a-0055d302498a</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>https://www.airbnb.com/experiences/3102714?currentTab=experience_tab&amp;federatedSearchId=526f5db2-2cae-4623-ac66-a5a254ae550c&amp;searchId=10e5ef69-49a1-4355-8dd6-d4fbd63addef&amp;sectionId=8d95b00f-bf58-4e5e-bb2a-cd27e7f450cc</t>
+          <t>https://www.airbnb.com/experiences/3102714?currentTab=experience_tab&amp;federatedSearchId=e74343bc-d4f2-44b5-bcbb-261b1bd0e7d3&amp;searchId=b06b2908-16d1-40ae-a1bb-0864f164d27b&amp;sectionId=7f116f53-1a8d-42d9-a67a-0055d302498a</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>https://www.airbnb.com/experiences/209002?currentTab=experience_tab&amp;federatedSearchId=526f5db2-2cae-4623-ac66-a5a254ae550c&amp;searchId=10e5ef69-49a1-4355-8dd6-d4fbd63addef&amp;sectionId=8d95b00f-bf58-4e5e-bb2a-cd27e7f450cc</t>
+          <t>https://www.airbnb.com/experiences/209002?currentTab=experience_tab&amp;federatedSearchId=e74343bc-d4f2-44b5-bcbb-261b1bd0e7d3&amp;searchId=b06b2908-16d1-40ae-a1bb-0864f164d27b&amp;sectionId=7f116f53-1a8d-42d9-a67a-0055d302498a</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>https://www.airbnb.com/experiences/3227484?currentTab=experience_tab&amp;federatedSearchId=526f5db2-2cae-4623-ac66-a5a254ae550c&amp;searchId=10e5ef69-49a1-4355-8dd6-d4fbd63addef&amp;sectionId=8d95b00f-bf58-4e5e-bb2a-cd27e7f450cc</t>
+          <t>https://www.airbnb.com/experiences/3227484?currentTab=experience_tab&amp;federatedSearchId=e74343bc-d4f2-44b5-bcbb-261b1bd0e7d3&amp;searchId=b06b2908-16d1-40ae-a1bb-0864f164d27b&amp;sectionId=7f116f53-1a8d-42d9-a67a-0055d302498a</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>https://www.airbnb.com/experiences/82265?currentTab=experience_tab&amp;federatedSearchId=526f5db2-2cae-4623-ac66-a5a254ae550c&amp;searchId=10e5ef69-49a1-4355-8dd6-d4fbd63addef&amp;sectionId=8d95b00f-bf58-4e5e-bb2a-cd27e7f450cc</t>
+          <t>https://www.airbnb.com/experiences/82265?currentTab=experience_tab&amp;federatedSearchId=e74343bc-d4f2-44b5-bcbb-261b1bd0e7d3&amp;searchId=b06b2908-16d1-40ae-a1bb-0864f164d27b&amp;sectionId=7f116f53-1a8d-42d9-a67a-0055d302498a</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>https://www.airbnb.com/experiences/1477782?currentTab=experience_tab&amp;federatedSearchId=526f5db2-2cae-4623-ac66-a5a254ae550c&amp;searchId=10e5ef69-49a1-4355-8dd6-d4fbd63addef&amp;sectionId=8d95b00f-bf58-4e5e-bb2a-cd27e7f450cc</t>
+          <t>https://www.airbnb.com/experiences/1477782?currentTab=experience_tab&amp;federatedSearchId=e74343bc-d4f2-44b5-bcbb-261b1bd0e7d3&amp;searchId=b06b2908-16d1-40ae-a1bb-0864f164d27b&amp;sectionId=7f116f53-1a8d-42d9-a67a-0055d302498a</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>https://www.airbnb.com/experiences/1497730?currentTab=experience_tab&amp;federatedSearchId=526f5db2-2cae-4623-ac66-a5a254ae550c&amp;searchId=10e5ef69-49a1-4355-8dd6-d4fbd63addef&amp;sectionId=8d95b00f-bf58-4e5e-bb2a-cd27e7f450cc</t>
+          <t>https://www.airbnb.com/experiences/1497730?currentTab=experience_tab&amp;federatedSearchId=e74343bc-d4f2-44b5-bcbb-261b1bd0e7d3&amp;searchId=b06b2908-16d1-40ae-a1bb-0864f164d27b&amp;sectionId=7f116f53-1a8d-42d9-a67a-0055d302498a</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>https://www.airbnb.com/experiences/872328?currentTab=experience_tab&amp;federatedSearchId=526f5db2-2cae-4623-ac66-a5a254ae550c&amp;searchId=10e5ef69-49a1-4355-8dd6-d4fbd63addef&amp;sectionId=8d95b00f-bf58-4e5e-bb2a-cd27e7f450cc</t>
+          <t>https://www.airbnb.com/experiences/872328?currentTab=experience_tab&amp;federatedSearchId=e74343bc-d4f2-44b5-bcbb-261b1bd0e7d3&amp;searchId=b06b2908-16d1-40ae-a1bb-0864f164d27b&amp;sectionId=7f116f53-1a8d-42d9-a67a-0055d302498a</t>
         </is>
       </c>
     </row>

</xml_diff>